<commit_message>
Cedulas resumen actualizadas a octubre 2020
</commit_message>
<xml_diff>
--- a/varios/ESTADO FINANCIERO PRELIMINAR  OCT2020 TELSOTERRA.xlsx
+++ b/varios/ESTADO FINANCIERO PRELIMINAR  OCT2020 TELSOTERRA.xlsx
@@ -1508,15 +1508,15 @@
   </sheetPr>
   <dimension ref="A1:BL230"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B207" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C233" activeCellId="0" sqref="C233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="2" width="10.71"/>
@@ -3030,7 +3030,7 @@
       <c r="D25" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="9" t="n">
         <v>37165.96</v>
       </c>
       <c r="K25" s="4"/>
@@ -3101,7 +3101,7 @@
       <c r="D26" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="9" t="n">
         <v>389.84</v>
       </c>
       <c r="K26" s="4"/>
@@ -3172,7 +3172,7 @@
       <c r="D27" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="9" t="n">
         <v>1128.42</v>
       </c>
       <c r="K27" s="4"/>
@@ -3319,7 +3319,7 @@
       <c r="D29" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="9" t="n">
         <v>0.01</v>
       </c>
       <c r="K29" s="4"/>
@@ -3390,7 +3390,7 @@
       <c r="D30" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="9" t="n">
         <v>286448.89</v>
       </c>
       <c r="K30" s="4"/>
@@ -3461,7 +3461,7 @@
       <c r="D31" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K31" s="4"/>
@@ -3532,7 +3532,7 @@
       <c r="D32" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="4"/>
@@ -3679,8 +3679,8 @@
       <c r="D34" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7" t="n">
+      <c r="E34" s="10"/>
+      <c r="F34" s="11" t="n">
         <v>950781.51</v>
       </c>
       <c r="G34" s="7"/>
@@ -3755,9 +3755,10 @@
       <c r="D35" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="9" t="n">
         <v>950781.51</v>
       </c>
+      <c r="F35" s="12"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -5798,7 +5799,7 @@
       <c r="D63" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="9" t="n">
         <v>93762.08</v>
       </c>
       <c r="K63" s="4"/>
@@ -5869,7 +5870,7 @@
       <c r="D64" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="E64" s="9" t="n">
         <v>171961.36</v>
       </c>
       <c r="K64" s="4"/>
@@ -6092,7 +6093,7 @@
       <c r="D67" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E67" s="1" t="n">
+      <c r="E67" s="9" t="n">
         <v>4084.44</v>
       </c>
       <c r="K67" s="4"/>
@@ -6467,7 +6468,7 @@
       <c r="D72" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E72" s="1" t="n">
+      <c r="E72" s="9" t="n">
         <v>1235119.31</v>
       </c>
       <c r="K72" s="4"/>
@@ -6538,7 +6539,7 @@
       <c r="D73" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E73" s="1" t="n">
+      <c r="E73" s="9" t="n">
         <v>3431.05</v>
       </c>
       <c r="K73" s="4"/>
@@ -6609,7 +6610,7 @@
       <c r="D74" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E74" s="1" t="n">
+      <c r="E74" s="9" t="n">
         <v>143989.65</v>
       </c>
       <c r="K74" s="4"/>
@@ -6680,7 +6681,7 @@
       <c r="D75" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="E75" s="6"/>
+      <c r="E75" s="10"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7" t="n">
         <v>-317891.9</v>
@@ -6756,7 +6757,7 @@
       <c r="D76" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E76" s="6"/>
+      <c r="E76" s="10"/>
       <c r="F76" s="7" t="n">
         <v>-317891.9</v>
       </c>
@@ -6832,7 +6833,7 @@
       <c r="D77" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E77" s="1" t="n">
+      <c r="E77" s="9" t="n">
         <v>-293543.06</v>
       </c>
       <c r="K77" s="4"/>
@@ -6903,7 +6904,7 @@
       <c r="D78" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E78" s="1" t="n">
+      <c r="E78" s="9" t="n">
         <v>-24348.84</v>
       </c>
       <c r="K78" s="4"/>
@@ -7354,7 +7355,7 @@
       <c r="D84" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E84" s="1" t="n">
+      <c r="E84" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K84" s="4"/>
@@ -7425,7 +7426,7 @@
       <c r="D85" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E85" s="1" t="n">
+      <c r="E85" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K85" s="4"/>
@@ -7496,7 +7497,7 @@
       <c r="D86" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E86" s="1" t="n">
+      <c r="E86" s="9" t="n">
         <v>-9636.94</v>
       </c>
       <c r="K86" s="4"/>
@@ -7567,7 +7568,7 @@
       <c r="D87" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E87" s="1" t="n">
+      <c r="E87" s="9" t="n">
         <v>-0.01</v>
       </c>
       <c r="K87" s="4"/>
@@ -7714,7 +7715,7 @@
       <c r="D89" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E89" s="1" t="n">
+      <c r="E89" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K89" s="4"/>
@@ -7785,7 +7786,7 @@
       <c r="D90" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E90" s="1" t="n">
+      <c r="E90" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K90" s="4"/>
@@ -7856,7 +7857,7 @@
       <c r="D91" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E91" s="1" t="n">
+      <c r="E91" s="9" t="n">
         <v>-2738.9</v>
       </c>
       <c r="K91" s="4"/>
@@ -7927,7 +7928,7 @@
       <c r="D92" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E92" s="1" t="n">
+      <c r="E92" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K92" s="4"/>
@@ -7998,7 +7999,7 @@
       <c r="D93" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E93" s="1" t="n">
+      <c r="E93" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K93" s="4"/>
@@ -8069,7 +8070,7 @@
       <c r="D94" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E94" s="1" t="n">
+      <c r="E94" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K94" s="4"/>
@@ -8292,7 +8293,7 @@
       <c r="D97" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E97" s="1" t="n">
+      <c r="E97" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K97" s="4"/>
@@ -8363,7 +8364,7 @@
       <c r="D98" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E98" s="1" t="n">
+      <c r="E98" s="9" t="n">
         <v>-2917.94</v>
       </c>
       <c r="K98" s="4"/>
@@ -8434,7 +8435,7 @@
       <c r="D99" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E99" s="1" t="n">
+      <c r="E99" s="9" t="n">
         <v>-2169.95</v>
       </c>
       <c r="K99" s="4"/>
@@ -8505,7 +8506,7 @@
       <c r="D100" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E100" s="1" t="n">
+      <c r="E100" s="9" t="n">
         <v>-20356</v>
       </c>
       <c r="K100" s="4"/>
@@ -8576,7 +8577,7 @@
       <c r="D101" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E101" s="1" t="n">
+      <c r="E101" s="9" t="n">
         <v>-4146.84</v>
       </c>
       <c r="K101" s="4"/>
@@ -8647,7 +8648,7 @@
       <c r="D102" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E102" s="1" t="n">
+      <c r="E102" s="9" t="n">
         <v>-657.15</v>
       </c>
       <c r="K102" s="4"/>
@@ -8718,7 +8719,7 @@
       <c r="D103" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E103" s="1" t="n">
+      <c r="E103" s="9" t="n">
         <v>-351.61</v>
       </c>
       <c r="K103" s="4"/>
@@ -8789,7 +8790,7 @@
       <c r="D104" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="E104" s="1" t="n">
+      <c r="E104" s="9" t="n">
         <v>-231683.36</v>
       </c>
       <c r="K104" s="4"/>
@@ -9012,7 +9013,7 @@
       <c r="D107" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E107" s="1" t="n">
+      <c r="E107" s="9" t="n">
         <v>-507080.34</v>
       </c>
     </row>
@@ -9073,7 +9074,7 @@
       <c r="D110" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E110" s="1" t="n">
+      <c r="E110" s="9" t="n">
         <v>-2500</v>
       </c>
     </row>
@@ -9134,7 +9135,7 @@
       <c r="D113" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E113" s="1" t="n">
+      <c r="E113" s="9" t="n">
         <v>-1029213.97</v>
       </c>
     </row>
@@ -9151,7 +9152,7 @@
       <c r="D114" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E114" s="1" t="n">
+      <c r="E114" s="9" t="n">
         <v>-4870</v>
       </c>
     </row>
@@ -9212,7 +9213,7 @@
       <c r="D117" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E117" s="1" t="n">
+      <c r="E117" s="9" t="n">
         <v>-65608.05</v>
       </c>
     </row>
@@ -9317,7 +9318,7 @@
       <c r="D122" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E122" s="1" t="n">
+      <c r="E122" s="9" t="n">
         <v>-1085.41</v>
       </c>
     </row>
@@ -9378,7 +9379,7 @@
       <c r="D125" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E125" s="1" t="n">
+      <c r="E125" s="9" t="n">
         <v>-1342257.54</v>
       </c>
     </row>
@@ -9820,7 +9821,7 @@
       <c r="D152" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E152" s="1" t="n">
+      <c r="E152" s="9" t="n">
         <v>-832663.43</v>
       </c>
     </row>
@@ -9947,7 +9948,7 @@
       <c r="D158" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E158" s="1" t="n">
+      <c r="E158" s="9" t="n">
         <v>62384.72</v>
       </c>
     </row>
@@ -9964,7 +9965,7 @@
       <c r="D159" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E159" s="6"/>
+      <c r="E159" s="10"/>
       <c r="F159" s="7" t="n">
         <v>37653.42</v>
       </c>
@@ -9986,7 +9987,7 @@
       <c r="D160" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E160" s="1" t="n">
+      <c r="E160" s="9" t="n">
         <v>37653.42</v>
       </c>
     </row>
@@ -10003,7 +10004,7 @@
       <c r="D161" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E161" s="6"/>
+      <c r="E161" s="10"/>
       <c r="F161" s="7" t="n">
         <v>17035.65</v>
       </c>
@@ -10025,7 +10026,7 @@
       <c r="D162" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E162" s="1" t="n">
+      <c r="E162" s="9" t="n">
         <v>17035.65</v>
       </c>
     </row>
@@ -10042,7 +10043,7 @@
       <c r="D163" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E163" s="6"/>
+      <c r="E163" s="10"/>
       <c r="F163" s="7" t="n">
         <v>86997.3</v>
       </c>
@@ -10064,7 +10065,7 @@
       <c r="D164" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E164" s="1" t="n">
+      <c r="E164" s="9" t="n">
         <v>86997.3</v>
       </c>
     </row>
@@ -11329,7 +11330,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="10.53"/>
   </cols>
@@ -11355,7 +11356,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="10.53"/>
   </cols>

</xml_diff>